<commit_message>
chore: dynamic charts and visual filters
</commit_message>
<xml_diff>
--- a/Xbox_Game_Pass_Subscriptions_Sales.xlsx
+++ b/Xbox_Game_Pass_Subscriptions_Sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Personal Projects\DIO\xbox-game-pass-subscriptions-salles-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA24E451-9C56-4F62-97FC-AE2DF7EEF783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA37EA2-DCBE-4086-8812-E48D72858208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
@@ -18,11 +18,22 @@
     <sheet name="Calculations" sheetId="3" r:id="rId3"/>
     <sheet name="D̳ashboard" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="Slicer_Subscription_Type">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="7" r:id="rId5"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId6"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -1227,9 +1238,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF5BF6A8"/>
       <color rgb="FF22C55E"/>
       <color rgb="FFE8E6E9"/>
-      <color rgb="FF5BF6A8"/>
       <color rgb="FF000000"/>
       <color rgb="FFE0E0E0"/>
       <color rgb="FFEDEDED"/>
@@ -1248,6 +1259,863 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Xbox_Game_Pass_Subscriptions_Sales.xlsx]Calculations!PivotTable2</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Calculations!$C$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5BF6A8"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calculations!$B$21:$B$23</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Yes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calculations!$C$21:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>_-"R$"\ * #,##0.00_-;\-"R$"\ * #,##0.00_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3BF5-4B0D-94C5-B7E8AEA6BE5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1591488639"/>
+        <c:axId val="1591502559"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1591488639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1591502559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1591502559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1591488639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1987,6 +2855,120 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4A272A4-BB25-C7E7-6700-263BFCEAECF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Subscription Type">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBE85526-70DF-4AE4-02CB-B238966FD232}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Subscription Type"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2948940" y="3108960"/>
+              <a:ext cx="1828800" cy="2581275"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2330,7 +3312,7 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="1867138719"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
@@ -6767,7 +7749,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73046DD2-38AA-484A-B28C-C17DCB1F2C20}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73046DD2-38AA-484A-B28C-C17DCB1F2C20}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B20:C23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -6822,11 +7804,22 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="6" item="0" hier="-1"/>
+    <pageField fld="6" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Total Value" fld="12" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -7183,6 +8176,29 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Subscription_Type" xr10:uid="{1290F47E-1F0F-4559-8DFB-BB8125B29902}" sourceName="Subscription Type">
+  <pivotTables>
+    <pivotTable tabId="3" name="PivotTable2"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1867138719">
+      <items count="3">
+        <i x="1"/>
+        <i x="0"/>
+        <i x="2" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Subscription Type" xr10:uid="{B7DC93E1-F303-4773-A6AD-9C822B764448}" cache="Slicer_Subscription_Type" caption="Subscription Type" style="SlicerStyleLight6" rowHeight="247650"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="13">
   <autoFilter ref="A1:M296" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}">
@@ -7533,8 +8549,8 @@
   </sheetPr>
   <dimension ref="B3:P21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19879,8 +20895,8 @@
   </sheetPr>
   <dimension ref="B3:C23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19967,7 +20983,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
@@ -19983,7 +20999,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="15">
-        <v>217</v>
+        <v>806</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
@@ -19991,7 +21007,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="15">
-        <v>1537</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
@@ -19999,13 +21015,20 @@
         <v>316</v>
       </c>
       <c r="C23" s="15">
-        <v>1754</v>
+        <v>2308</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
   <drawing r:id="rId4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId5"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
chore: organize and style the dashboard area
</commit_message>
<xml_diff>
--- a/Xbox_Game_Pass_Subscriptions_Sales.xlsx
+++ b/Xbox_Game_Pass_Subscriptions_Sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Personal Projects\DIO\xbox-game-pass-subscriptions-salles-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D12E2BA-C47D-4D78-8CC8-5ECBA2B392B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3284B19B-C18C-4D00-9206-66753CDEE61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
     <sheet name="A̳ssets" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="321">
   <si>
     <t>Paleta de Cores</t>
   </si>
@@ -1051,15 +1052,18 @@
       <t>( contendo todas as assinaturas agregadas )</t>
     </r>
   </si>
+  <si>
+    <t>XBOX GAME PASS SUBSCRIPTION SALLES</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1086,6 +1090,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF22C55E"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1135,7 +1147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1152,13 +1164,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1185,13 +1206,56 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF22C55E"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9"/>
+        </left>
+        <right style="thin">
+          <color theme="9"/>
+        </right>
+        <top style="thin">
+          <color theme="9"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1235,24 +1299,742 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="SlicerStyleLight6 2" pivot="0" table="0" count="10" xr9:uid="{313518BB-6A92-4C63-A7C1-F9886D7ADFD5}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF22C55E"/>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FF2AE6B1"/>
+      <color rgb="FFE8E6E9"/>
       <color rgb="FF5BF6A8"/>
-      <color rgb="FF22C55E"/>
-      <color rgb="FFE8E6E9"/>
       <color rgb="FF000000"/>
       <color rgb="FFE0E0E0"/>
       <color rgb="FFEDEDED"/>
       <color rgb="FFF7F8FC"/>
-      <color rgb="FF2AE6B1"/>
       <color rgb="FF9BC848"/>
-      <color rgb="FFE70011"/>
     </mruColors>
   </colors>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{46F421CA-312F-682f-3DD2-61675219B42D}">
+      <x14:dxfs count="24">
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.79998168889431442"/>
+              <bgColor theme="9" tint="0.79998168889431442"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.59999389629810485"/>
+              <bgColor theme="9" tint="0.59999389629810485"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFE0E0E0"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFE0E0E0"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFE0E0E0"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFE0E0E0"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.79998168889431442"/>
+              <bgColor theme="9" tint="0.79998168889431442"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.59999389629810485"/>
+              <bgColor theme="9" tint="0.59999389629810485"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFE0E0E0"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFE0E0E0"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFE0E0E0"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFE0E0E0"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <gradientFill degree="90">
+              <stop position="0">
+                <color rgb="FFF8E162"/>
+              </stop>
+              <stop position="1">
+                <color rgb="FFFCF7E0"/>
+              </stop>
+            </gradientFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.79998168889431442"/>
+              <bgColor theme="9" tint="0.79998168889431442"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor theme="9" tint="0.59999389629810485"/>
+              <bgColor theme="9" tint="0.59999389629810485"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FF999999"/>
+            </left>
+            <right style="thin">
+              <color rgb="FF999999"/>
+            </right>
+            <top style="thin">
+              <color rgb="FF999999"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FF999999"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF828282"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFE0E0E0"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFE0E0E0"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFE0E0E0"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFE0E0E0"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+        <dxf>
+          <font>
+            <color rgb="FF000000"/>
+          </font>
+          <fill>
+            <patternFill patternType="solid">
+              <fgColor rgb="FFFFFFFF"/>
+              <bgColor rgb="FFFFFFFF"/>
+            </patternFill>
+          </fill>
+          <border>
+            <left style="thin">
+              <color rgb="FFCCCCCC"/>
+            </left>
+            <right style="thin">
+              <color rgb="FFCCCCCC"/>
+            </right>
+            <top style="thin">
+              <color rgb="FFCCCCCC"/>
+            </top>
+            <bottom style="thin">
+              <color rgb="FFCCCCCC"/>
+            </bottom>
+            <vertical/>
+            <horizontal/>
+          </border>
+        </dxf>
+      </x14:dxfs>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1">
+        <x14:slicerStyle name="SlicerStyleLight6 2">
+          <x14:slicerStyleElements>
+            <x14:slicerStyleElement type="unselectedItemWithData" dxfId="7"/>
+            <x14:slicerStyleElement type="unselectedItemWithNoData" dxfId="6"/>
+            <x14:slicerStyleElement type="selectedItemWithData" dxfId="5"/>
+            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="4"/>
+            <x14:slicerStyleElement type="hoveredUnselectedItemWithData" dxfId="3"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithData" dxfId="2"/>
+            <x14:slicerStyleElement type="hoveredUnselectedItemWithNoData" dxfId="1"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithNoData" dxfId="0"/>
+          </x14:slicerStyleElements>
+        </x14:slicerStyle>
+      </x14:slicerStyles>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
@@ -1276,7 +2058,7 @@
   </mc:AlternateContent>
   <c:pivotSource>
     <c:name>[Xbox_Game_Pass_Subscriptions_Sales.xlsx]Calculations!PivotTable2</c:name>
-    <c:fmtId val="1"/>
+    <c:fmtId val="6"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
@@ -1313,6 +2095,118 @@
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="5BF6A8"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
             <a:srgbClr val="5BF6A8"/>
@@ -1419,17 +2313,17 @@
                 <c:formatCode>_-"R$"\ * #,##0.00_-;\-"R$"\ * #,##0.00_-;_-"R$"\ * "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>806</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1502</c:v>
+                  <c:v>1537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3BF5-4B0D-94C5-B7E8AEA6BE5D}"/>
+              <c16:uniqueId val="{00000000-5617-4980-A17B-BBB86CE79363}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1531,9 +2425,7 @@
     </c:extLst>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
       <a:round/>
@@ -2855,63 +3747,194 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1257301</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50673</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4A272A4-BB25-C7E7-6700-263BFCEAECF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDB97C64-D137-4D5C-A992-A9D38E584DEA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="8911" r="73597"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="180975"/>
+          <a:ext cx="504826" cy="984123"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2019300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>20955</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C20CFEAE-B255-4297-C78C-DB35E15EB4A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2571751" y="2181225"/>
+          <a:ext cx="4838700" cy="2943225"/>
+          <a:chOff x="2781301" y="2238375"/>
+          <a:chExt cx="4838700" cy="2943225"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Rectangle: Rounded Corners 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6A17D16-3DD3-F8D8-48F1-A9C566B40CBF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2781301" y="2238375"/>
+            <a:ext cx="4838700" cy="2932345"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 4703"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="5" name="Chart 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82A1D974-93BE-4814-A46E-01F0C5A75E28}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr>
+            <a:graphicFrameLocks/>
+          </xdr:cNvGraphicFramePr>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="3011805" y="2438400"/>
+          <a:ext cx="4572000" cy="2743200"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>116205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1971675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="Subscription Type">
+            <xdr:cNvPr id="6" name="Subscription Type">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBE85526-70DF-4AE4-02CB-B238966FD232}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38EB29BA-F3C3-4688-89C9-6555BFB05331}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2938,7 +3961,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2948940" y="3108960"/>
+              <a:off x="142875" y="2392680"/>
               <a:ext cx="1828800" cy="2581275"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7749,7 +8772,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73046DD2-38AA-484A-B28C-C17DCB1F2C20}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73046DD2-38AA-484A-B28C-C17DCB1F2C20}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="B20:C23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -7804,13 +8827,22 @@
     <i/>
   </colItems>
   <pageFields count="1">
-    <pageField fld="6" item="2" hier="-1"/>
+    <pageField fld="6" item="0" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Total Value" fld="12" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="2">
     <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="2" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -7833,7 +8865,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7CA51761-CCD9-4D01-A266-DB665D99DC92}" name="tbl_annual_total" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7CA51761-CCD9-4D01-A266-DB665D99DC92}" name="tbl_annual_total" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B9:C13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -8177,16 +9209,16 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Subscription_Type" xr10:uid="{1290F47E-1F0F-4559-8DFB-BB8125B29902}" sourceName="Subscription Type">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Subscription_Type" xr10:uid="{D82268F0-43BC-46B7-8355-6B302FB9582A}" sourceName="Subscription Type">
   <pivotTables>
     <pivotTable tabId="3" name="PivotTable2"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1867138719">
       <items count="3">
-        <i x="1"/>
+        <i x="1" s="1"/>
         <i x="0"/>
-        <i x="2" s="1"/>
+        <i x="2"/>
       </items>
     </tabular>
   </data>
@@ -8195,12 +9227,12 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <slicer name="Subscription Type" xr10:uid="{B7DC93E1-F303-4773-A6AD-9C822B764448}" cache="Slicer_Subscription_Type" caption="Subscription Type" style="SlicerStyleLight6" rowHeight="247650"/>
+  <slicer name="Subscription Type" xr10:uid="{60585E00-B150-4915-B593-597CE9BB7EC5}" cache="Slicer_Subscription_Type" caption="Subscription Type" style="SlicerStyleLight6 2" rowHeight="247650"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:M296" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="A1:M296" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}">
     <filterColumn colId="7">
       <filters>
@@ -8209,19 +9241,19 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8550,7 +9582,7 @@
   <dimension ref="B3:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20895,8 +21927,8 @@
   </sheetPr>
   <dimension ref="B3:C23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20983,7 +22015,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
@@ -20999,7 +22031,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="15">
-        <v>806</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
@@ -21007,7 +22039,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="15">
-        <v>1502</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
@@ -21015,62 +22047,840 @@
         <v>316</v>
       </c>
       <c r="C23" s="15">
-        <v>2308</v>
+        <v>1754</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
   <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210F14EF-C0B7-459D-9E09-3130BA4314A6}">
+  <dimension ref="A1:O259"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="41.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:15" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:15" ht="37.200000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:15" s="7" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" s="7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" s="7" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" s="7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="O13" s="18"/>
+    </row>
+    <row r="14" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="4"/>
+    </row>
+    <row r="71" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="4"/>
+    </row>
+    <row r="75" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="4"/>
+    </row>
+    <row r="83" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="4"/>
+    </row>
+    <row r="84" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="4"/>
+    </row>
+    <row r="85" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="4"/>
+    </row>
+    <row r="92" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="4"/>
+    </row>
+    <row r="93" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="4"/>
+    </row>
+    <row r="94" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="4"/>
+    </row>
+    <row r="95" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="4"/>
+    </row>
+    <row r="96" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="4"/>
+    </row>
+    <row r="97" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="4"/>
+    </row>
+    <row r="98" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="4"/>
+    </row>
+    <row r="99" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="4"/>
+    </row>
+    <row r="100" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="4"/>
+    </row>
+    <row r="101" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="4"/>
+    </row>
+    <row r="102" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="4"/>
+    </row>
+    <row r="103" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="4"/>
+    </row>
+    <row r="104" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="4"/>
+    </row>
+    <row r="105" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="4"/>
+    </row>
+    <row r="106" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="4"/>
+    </row>
+    <row r="107" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="4"/>
+    </row>
+    <row r="108" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="4"/>
+    </row>
+    <row r="109" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="4"/>
+    </row>
+    <row r="110" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="4"/>
+    </row>
+    <row r="111" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="4"/>
+    </row>
+    <row r="112" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="4"/>
+    </row>
+    <row r="113" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="4"/>
+    </row>
+    <row r="114" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="4"/>
+    </row>
+    <row r="115" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="4"/>
+    </row>
+    <row r="116" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="4"/>
+    </row>
+    <row r="117" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="4"/>
+    </row>
+    <row r="118" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="4"/>
+    </row>
+    <row r="119" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="4"/>
+    </row>
+    <row r="120" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="4"/>
+    </row>
+    <row r="121" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="4"/>
+    </row>
+    <row r="122" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="4"/>
+    </row>
+    <row r="123" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="4"/>
+    </row>
+    <row r="124" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="4"/>
+    </row>
+    <row r="125" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="4"/>
+    </row>
+    <row r="126" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="4"/>
+    </row>
+    <row r="127" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="4"/>
+    </row>
+    <row r="128" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="4"/>
+    </row>
+    <row r="129" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="4"/>
+    </row>
+    <row r="130" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="4"/>
+    </row>
+    <row r="131" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="4"/>
+    </row>
+    <row r="132" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="4"/>
+    </row>
+    <row r="133" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="4"/>
+    </row>
+    <row r="134" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="4"/>
+    </row>
+    <row r="135" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="4"/>
+    </row>
+    <row r="136" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="4"/>
+    </row>
+    <row r="137" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="4"/>
+    </row>
+    <row r="138" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="4"/>
+    </row>
+    <row r="139" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="4"/>
+    </row>
+    <row r="140" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="4"/>
+    </row>
+    <row r="141" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="4"/>
+    </row>
+    <row r="142" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="4"/>
+    </row>
+    <row r="143" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="4"/>
+    </row>
+    <row r="144" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="4"/>
+    </row>
+    <row r="145" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="4"/>
+    </row>
+    <row r="146" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="4"/>
+    </row>
+    <row r="147" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="4"/>
+    </row>
+    <row r="148" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="4"/>
+    </row>
+    <row r="149" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="4"/>
+    </row>
+    <row r="150" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="4"/>
+    </row>
+    <row r="151" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="4"/>
+    </row>
+    <row r="152" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="4"/>
+    </row>
+    <row r="153" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="4"/>
+    </row>
+    <row r="154" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="4"/>
+    </row>
+    <row r="155" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="4"/>
+    </row>
+    <row r="156" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="4"/>
+    </row>
+    <row r="157" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="4"/>
+    </row>
+    <row r="158" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="4"/>
+    </row>
+    <row r="159" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="4"/>
+    </row>
+    <row r="160" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="4"/>
+    </row>
+    <row r="161" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="4"/>
+    </row>
+    <row r="162" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="4"/>
+    </row>
+    <row r="163" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="4"/>
+    </row>
+    <row r="164" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="4"/>
+    </row>
+    <row r="165" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="4"/>
+    </row>
+    <row r="166" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="4"/>
+    </row>
+    <row r="167" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="4"/>
+    </row>
+    <row r="168" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="4"/>
+    </row>
+    <row r="169" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="4"/>
+    </row>
+    <row r="170" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="4"/>
+    </row>
+    <row r="171" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="4"/>
+    </row>
+    <row r="172" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="4"/>
+    </row>
+    <row r="173" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="4"/>
+    </row>
+    <row r="174" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="4"/>
+    </row>
+    <row r="175" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="4"/>
+    </row>
+    <row r="176" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="4"/>
+    </row>
+    <row r="177" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="4"/>
+    </row>
+    <row r="178" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="4"/>
+    </row>
+    <row r="179" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="4"/>
+    </row>
+    <row r="180" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="4"/>
+    </row>
+    <row r="181" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="4"/>
+    </row>
+    <row r="182" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="4"/>
+    </row>
+    <row r="183" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="4"/>
+    </row>
+    <row r="184" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="4"/>
+    </row>
+    <row r="185" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="4"/>
+    </row>
+    <row r="186" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="4"/>
+    </row>
+    <row r="187" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="4"/>
+    </row>
+    <row r="188" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="4"/>
+    </row>
+    <row r="189" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="4"/>
+    </row>
+    <row r="190" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="4"/>
+    </row>
+    <row r="191" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="4"/>
+    </row>
+    <row r="192" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="4"/>
+    </row>
+    <row r="193" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="4"/>
+    </row>
+    <row r="194" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="4"/>
+    </row>
+    <row r="195" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="4"/>
+    </row>
+    <row r="196" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="4"/>
+    </row>
+    <row r="197" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="4"/>
+    </row>
+    <row r="198" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="4"/>
+    </row>
+    <row r="199" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="4"/>
+    </row>
+    <row r="200" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="4"/>
+    </row>
+    <row r="201" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="4"/>
+    </row>
+    <row r="202" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="4"/>
+    </row>
+    <row r="203" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="4"/>
+    </row>
+    <row r="204" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="4"/>
+    </row>
+    <row r="205" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="4"/>
+    </row>
+    <row r="206" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="4"/>
+    </row>
+    <row r="207" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="4"/>
+    </row>
+    <row r="208" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="4"/>
+    </row>
+    <row r="209" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="4"/>
+    </row>
+    <row r="210" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="4"/>
+    </row>
+    <row r="211" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="4"/>
+    </row>
+    <row r="212" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="4"/>
+    </row>
+    <row r="213" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="4"/>
+    </row>
+    <row r="214" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="4"/>
+    </row>
+    <row r="215" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="4"/>
+    </row>
+    <row r="216" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="4"/>
+    </row>
+    <row r="217" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="4"/>
+    </row>
+    <row r="218" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="4"/>
+    </row>
+    <row r="219" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="4"/>
+    </row>
+    <row r="220" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="4"/>
+    </row>
+    <row r="221" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="4"/>
+    </row>
+    <row r="222" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="4"/>
+    </row>
+    <row r="223" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="4"/>
+    </row>
+    <row r="224" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="4"/>
+    </row>
+    <row r="225" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="4"/>
+    </row>
+    <row r="226" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="4"/>
+    </row>
+    <row r="227" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="4"/>
+    </row>
+    <row r="228" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="4"/>
+    </row>
+    <row r="229" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="4"/>
+    </row>
+    <row r="230" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="4"/>
+    </row>
+    <row r="231" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="4"/>
+    </row>
+    <row r="232" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="4"/>
+    </row>
+    <row r="233" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="4"/>
+    </row>
+    <row r="234" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="4"/>
+    </row>
+    <row r="235" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="4"/>
+    </row>
+    <row r="236" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="4"/>
+    </row>
+    <row r="237" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="4"/>
+    </row>
+    <row r="238" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="4"/>
+    </row>
+    <row r="239" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="4"/>
+    </row>
+    <row r="240" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="4"/>
+    </row>
+    <row r="241" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="4"/>
+    </row>
+    <row r="242" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="4"/>
+    </row>
+    <row r="243" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="4"/>
+    </row>
+    <row r="244" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="4"/>
+    </row>
+    <row r="245" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="4"/>
+    </row>
+    <row r="246" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="4"/>
+    </row>
+    <row r="247" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A247" s="4"/>
+    </row>
+    <row r="248" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="4"/>
+    </row>
+    <row r="249" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="4"/>
+    </row>
+    <row r="250" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="4"/>
+    </row>
+    <row r="251" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="4"/>
+    </row>
+    <row r="252" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A252" s="4"/>
+    </row>
+    <row r="253" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A253" s="4"/>
+    </row>
+    <row r="254" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A254" s="4"/>
+    </row>
+    <row r="255" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A255" s="4"/>
+    </row>
+    <row r="256" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="4"/>
+    </row>
+    <row r="257" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A257" s="4"/>
+    </row>
+    <row r="258" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="4"/>
+    </row>
+    <row r="259" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A259" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
       <x14:slicerList>
-        <x14:slicer r:id="rId5"/>
+        <x14:slicer r:id="rId2"/>
       </x14:slicerList>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210F14EF-C0B7-459D-9E09-3130BA4314A6}">
-  <dimension ref="A2:A7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21232,6 +23042,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -21243,14 +23061,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>